<commit_message>
correct HFP for alex+jamie
</commit_message>
<xml_diff>
--- a/examples/HFP_alex+jamie.xlsx
+++ b/examples/HFP_alex+jamie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdlacasse/Owl/examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\MyProject\Owl\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC897897-090B-4B44-93ED-F035A36CFD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FCEE64-3D12-4FDA-A8BF-C42CBFD67DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="19420" windowHeight="11500" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="-28920" yWindow="12735" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Alex" sheetId="1" r:id="rId1"/>
@@ -492,28 +492,28 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2021</v>
       </c>
@@ -557,7 +557,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2022</v>
       </c>
@@ -572,7 +572,7 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -587,7 +587,7 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2024</v>
       </c>
@@ -602,7 +602,7 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -619,7 +619,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -636,7 +636,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -653,7 +653,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -670,7 +670,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -685,7 +685,7 @@
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -698,7 +698,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2031</v>
       </c>
@@ -711,7 +711,7 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2032</v>
       </c>
@@ -724,7 +724,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2033</v>
       </c>
@@ -737,7 +737,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2034</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2035</v>
       </c>
@@ -763,7 +763,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2036</v>
       </c>
@@ -776,7 +776,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2037</v>
       </c>
@@ -789,7 +789,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2038</v>
       </c>
@@ -802,7 +802,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2039</v>
       </c>
@@ -815,7 +815,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2040</v>
       </c>
@@ -828,7 +828,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2041</v>
       </c>
@@ -841,7 +841,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2042</v>
       </c>
@@ -854,7 +854,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2043</v>
       </c>
@@ -867,7 +867,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2044</v>
       </c>
@@ -880,7 +880,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2045</v>
       </c>
@@ -893,7 +893,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2046</v>
       </c>
@@ -906,7 +906,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2047</v>
       </c>
@@ -919,7 +919,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2048</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2049</v>
       </c>
@@ -945,7 +945,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2050</v>
       </c>
@@ -958,7 +958,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2051</v>
       </c>
@@ -971,7 +971,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2052</v>
       </c>
@@ -984,7 +984,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2053</v>
       </c>
@@ -997,7 +997,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2054</v>
       </c>
@@ -1010,7 +1010,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2055</v>
       </c>
@@ -1037,20 +1037,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.1640625" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>2021</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2022</v>
       </c>
@@ -1109,7 +1109,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2023</v>
       </c>
@@ -1124,7 +1124,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>2024</v>
       </c>
@@ -1139,7 +1139,7 @@
       </c>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -1154,7 +1154,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -1169,7 +1169,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2027</v>
       </c>
@@ -1184,7 +1184,7 @@
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -1199,7 +1199,7 @@
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2029</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2030</v>
       </c>
@@ -1225,7 +1225,7 @@
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2031</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2032</v>
       </c>
@@ -1251,7 +1251,7 @@
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2033</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2034</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2035</v>
       </c>
@@ -1290,7 +1290,7 @@
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2036</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2037</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2038</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2039</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2040</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2041</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2042</v>
       </c>
@@ -1381,7 +1381,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2043</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2044</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2045</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2046</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2047</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2048</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2049</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2050</v>
       </c>
@@ -1485,7 +1485,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2051</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2052</v>
       </c>
@@ -1511,7 +1511,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2053</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2054</v>
       </c>
@@ -1537,7 +1537,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2055</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2056</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2057</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2058</v>
       </c>
@@ -1594,18 +1594,18 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.5" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="1" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1660,21 +1660,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29335860-5C91-4189-B35F-4DDEB06D1DBA}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="b">
         <v>1</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>3.5</v>
       </c>
       <c r="H2">
-        <v>2045</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>5</v>

</xml_diff>

<commit_message>
HFP reproducibility and consistency fixes
- Edited values fix: Only reset timeListsFileName from 'edited values' to
  HFP_{caseName}.xlsx when the user actually downloads the HFP workbook,
  not when merely viewing the Reports page. Add markHFPAsSaved() and call
  it on download button click; rerun page to show updated state.

- Rename 'other inc.' to 'other inc' for consistency with other column
  headers. Add backward compatibility: HFP files with 'other inc.' are
  normalized when read. Update add_other_inc_column script and migrate
  example HFP files.
</commit_message>
<xml_diff>
--- a/examples/HFP_alex+jamie.xlsx
+++ b/examples/HFP_alex+jamie.xlsx
@@ -449,7 +449,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>other inc.</t>
+          <t>other inc</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>other inc.</t>
+          <t>other inc</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">

</xml_diff>